<commit_message>
Allow for more complex rules for data selection and add test function.
</commit_message>
<xml_diff>
--- a/tests/test_data/fakeData4Testing2.xlsx
+++ b/tests/test_data/fakeData4Testing2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munsky/Dropbox/GitHub/SSIT/tests/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munsky/Dropbox/GitHub/SSIT/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A66C1D9-6114-024B-B0AA-B9C148D8F1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96EE1FA-9D8A-DE48-990B-BCE5B0C6C543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24360" yWindow="8060" windowWidth="27640" windowHeight="16940" xr2:uid="{634C28CD-A18A-C84A-BAA7-147CB736806C}"/>
+    <workbookView xWindow="23560" yWindow="8060" windowWidth="27640" windowHeight="16940" xr2:uid="{634C28CD-A18A-C84A-BAA7-147CB736806C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>CellID</t>
   </si>
@@ -57,7 +57,13 @@
     <t>total</t>
   </si>
   <si>
-    <t>a</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>ab</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -541,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -637,7 +643,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>3</v>

</xml_diff>

<commit_message>
Update data in object to refer to filtered data.
</commit_message>
<xml_diff>
--- a/tests/test_data/fakeData4Testing2.xlsx
+++ b/tests/test_data/fakeData4Testing2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munsky/Dropbox/GitHub/SSIT/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96EE1FA-9D8A-DE48-990B-BCE5B0C6C543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F1F580-91E1-D346-BA5D-F9CE5B11C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23560" yWindow="8060" windowWidth="27640" windowHeight="16940" xr2:uid="{634C28CD-A18A-C84A-BAA7-147CB736806C}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,14 +652,14 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>